<commit_message>
[imp]修改密码策略 code 为 HZERO-PLATFORM
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/init-data/hzero_platform/hzero_platform/hzero-platform-oauth.xlsx
+++ b/src/main/resources/script/db/init-data/hzero_platform/hzero_platform/hzero-platform-oauth.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\WorkDev\hzero-resource\init-data\hzero-platform\hzero_platform\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projcect\hzero-platform\src\main\resources\script\db\init-data\hzero_platform\hzero_platform\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018375A4-1331-493A-83ED-10255F1D8FBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28695" windowHeight="14220" tabRatio="597" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="597" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -2273,9 +2274,6 @@
     <t>force_modify_password</t>
   </si>
   <si>
-    <t>HZERO</t>
-  </si>
-  <si>
     <t>admin1234</t>
   </si>
   <si>
@@ -2289,12 +2287,15 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>HZERO-PLATFORM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="48">
     <font>
       <sz val="12"/>
@@ -2832,7 +2833,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 2" xfId="1"/>
+    <cellStyle name="常规 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
@@ -3172,7 +3173,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3413,10 +3414,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
@@ -3677,7 +3678,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3846,10 +3847,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AD8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25"/>
   <sheetData>
@@ -3975,7 +3978,7 @@
         <v>70</v>
       </c>
       <c r="F8" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="G8" t="s">
         <v>104</v>
@@ -3984,16 +3987,16 @@
         <v>72</v>
       </c>
       <c r="I8" t="s">
+        <v>142</v>
+      </c>
+      <c r="J8" t="s">
         <v>143</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>144</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>145</v>
-      </c>
-      <c r="L8" t="s">
-        <v>146</v>
       </c>
       <c r="M8" t="s">
         <v>72</v>
@@ -4029,7 +4032,7 @@
         <v>76</v>
       </c>
       <c r="Y8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="Z8" t="s">
         <v>76</v>

</xml_diff>